<commit_message>
Updated ProductBacklog and SprintBacklog
</commit_message>
<xml_diff>
--- a/Documents/Deliverable_4/CSwap_Deliverable_4_ProductBacklog.xlsx
+++ b/Documents/Deliverable_4/CSwap_Deliverable_4_ProductBacklog.xlsx
@@ -5,18 +5,28 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tonyc\Documents\GitHub\COS420_Project\Documents\Deliverable_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Github\COS420_Project\Documents\Deliverable_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFF154E-F23E-4856-8E90-66F99E6330A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5586E9C1-B2F1-41A3-BA7A-05A034FC2429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7970" yWindow="2290" windowWidth="28800" windowHeight="17030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjHmi+eQAS38vJPXohR8+s/H+DMJw=="/>
     </ext>
@@ -136,7 +146,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,6 +210,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -260,7 +276,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -300,6 +316,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -565,21 +584,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.58203125" customWidth="1"/>
-    <col min="2" max="2" width="71.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.75" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="27.58203125" customWidth="1"/>
-    <col min="6" max="6" width="23.75" customWidth="1"/>
+    <col min="1" max="1" width="10.59765625" customWidth="1"/>
+    <col min="2" max="2" width="71.296875" customWidth="1"/>
+    <col min="3" max="3" width="22.69921875" customWidth="1"/>
+    <col min="4" max="4" width="26.296875" customWidth="1"/>
+    <col min="5" max="5" width="27.59765625" customWidth="1"/>
+    <col min="6" max="6" width="23.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,7 +618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -619,7 +638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -639,7 +658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -659,7 +678,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -679,7 +698,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -699,11 +718,11 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="5">
@@ -712,14 +731,14 @@
       <c r="D7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>34</v>
+      <c r="E7" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="F7" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -739,7 +758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -752,14 +771,14 @@
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>11</v>
+      <c r="E9" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="F9" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -779,7 +798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -792,18 +811,18 @@
       <c r="D11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>11</v>
+      <c r="E11" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="F11" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="9">
@@ -812,14 +831,14 @@
       <c r="D12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>11</v>
+      <c r="E12" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="F12" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -839,7 +858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -852,14 +871,14 @@
       <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>11</v>
+      <c r="E14" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="F14" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -879,7 +898,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -899,7 +918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -919,7 +938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -939,7 +958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -959,7 +978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -979,7 +998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -999,7 +1018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -1019,7 +1038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -1039,7 +1058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -1059,7 +1078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>23</v>
       </c>

</xml_diff>